<commit_message>
Add aprox. 50 words from at room on 19 jan 2012
</commit_message>
<xml_diff>
--- a/Vocabulares.xlsx
+++ b/Vocabulares.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="200">
   <si>
     <t>Word</t>
   </si>
@@ -46,13 +46,583 @@
   </si>
   <si>
     <t>अग्रणी</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 quiet girl </t>
+  </si>
+  <si>
+    <t>1 quiet girls teebra chal rahi thi mere aage-2</t>
+  </si>
+  <si>
+    <t>chrome nicky</t>
+  </si>
+  <si>
+    <t>nicky google chrome ko use karte -2 purani ho gayi.</t>
+  </si>
+  <si>
+    <t>paya+neer(water)</t>
+  </si>
+  <si>
+    <t>meni neer pane me agraani hau.</t>
+  </si>
+  <si>
+    <t>Aback</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>meri back me peeche se kesni danda mara tha.</t>
+  </si>
+  <si>
+    <t>Abandon</t>
+  </si>
+  <si>
+    <t>give up</t>
+  </si>
+  <si>
+    <t>abe+DON</t>
+  </si>
+  <si>
+    <t>peeche(H)</t>
+  </si>
+  <si>
+    <t>Abate</t>
+  </si>
+  <si>
+    <t>make less</t>
+  </si>
+  <si>
+    <t>aa+bat laga</t>
+  </si>
+  <si>
+    <t>Aa 550 bat lagaata hai ke tu use less (kam) kar dega</t>
+  </si>
+  <si>
+    <t>Abbreviate</t>
+  </si>
+  <si>
+    <t>a+veer+wait</t>
+  </si>
+  <si>
+    <t>संक्षिप्त करना</t>
+  </si>
+  <si>
+    <t>A veer wait kar raha hai vo tujhe aaj संक्षिप्त  me aacche se samjha dega</t>
+  </si>
+  <si>
+    <t>Abduct</t>
+  </si>
+  <si>
+    <t>kidnap</t>
+  </si>
+  <si>
+    <t>Adult+Doc</t>
+  </si>
+  <si>
+    <t>Adult (girl) doc ke kidnap karne wale ko 5 lacks melange. This is published in news paper</t>
+  </si>
+  <si>
+    <t>Diminish</t>
+  </si>
+  <si>
+    <t>कम</t>
+  </si>
+  <si>
+    <t>daamani+shy</t>
+  </si>
+  <si>
+    <t>daamani कम shy karti hai esileya bo fluient english seekh paayi hai.</t>
+  </si>
+  <si>
+    <t>Abhor</t>
+  </si>
+  <si>
+    <t>घृणा करना</t>
+  </si>
+  <si>
+    <t>Ab+bhor(morning)</t>
+  </si>
+  <si>
+    <t>Bhor ke baad sone waalon se meri maa घृणा  karti hai.</t>
+  </si>
+  <si>
+    <t>abide</t>
+  </si>
+  <si>
+    <t>Continue,remain</t>
+  </si>
+  <si>
+    <t>1+bite</t>
+  </si>
+  <si>
+    <t>Khaana etna testy tha ke me 1 bite kaane ke baad se jab tak bo khatam nahi ho gaya me CONTINUE karta raha</t>
+  </si>
+  <si>
+    <t>Abject</t>
+  </si>
+  <si>
+    <t>नीच</t>
+  </si>
+  <si>
+    <t>jet airo plane</t>
+  </si>
+  <si>
+    <t>Jet airo plane to khareed leya parntu bo etna नीच hai ke usme apni gareeb maa-baap ko bhi nai baithne deta</t>
+  </si>
+  <si>
+    <t>abnegation</t>
+  </si>
+  <si>
+    <t>इनकार</t>
+  </si>
+  <si>
+    <t>negation</t>
+  </si>
+  <si>
+    <t>usene itni NEGOSATION se shopkeepar ne use jeans sell karne he इनकार kar deya</t>
+  </si>
+  <si>
+    <t>निवासस्थान</t>
+  </si>
+  <si>
+    <t>adobi</t>
+  </si>
+  <si>
+    <t>Adobi ka निवासस्थान shaandar hai</t>
+  </si>
+  <si>
+    <t>abode</t>
+  </si>
+  <si>
+    <t>abolish</t>
+  </si>
+  <si>
+    <t>समाप्त करना</t>
+  </si>
+  <si>
+    <t>polish</t>
+  </si>
+  <si>
+    <t>ae mochi jaldi se समाप्त kar mujhe deer ho rahi hai</t>
+  </si>
+  <si>
+    <t>abominable</t>
+  </si>
+  <si>
+    <t>घिनौना</t>
+  </si>
+  <si>
+    <t>momelal</t>
+  </si>
+  <si>
+    <t>mujhe momelal  घिनौना lagta hai</t>
+  </si>
+  <si>
+    <t>detestable</t>
+  </si>
+  <si>
+    <t>dabaayi+test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dabaayi ka test mujhe घिनौना lagta hai </t>
+  </si>
+  <si>
+    <t>Abort</t>
+  </si>
+  <si>
+    <t>गर्भपात होना</t>
+  </si>
+  <si>
+    <t>bo+raat</t>
+  </si>
+  <si>
+    <t>bo raat aaj bhi yaad hai jab uska गर्भपात hua tha</t>
+  </si>
+  <si>
+    <t>abortion</t>
+  </si>
+  <si>
+    <t>गर्भपात</t>
+  </si>
+  <si>
+    <t>ab+or+paresaan</t>
+  </si>
+  <si>
+    <t>गर्भपात karke ab or paresaan mat  karna please</t>
+  </si>
+  <si>
+    <t>abrupt</t>
+  </si>
+  <si>
+    <t>आकस्मिक</t>
+  </si>
+  <si>
+    <t>bru (coffiiee)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bru coffiiee ka cap dekh kar me आकस्मिक me rah gaya </t>
+  </si>
+  <si>
+    <t>Absolve</t>
+  </si>
+  <si>
+    <t>दोषमुक्त करना</t>
+  </si>
+  <si>
+    <t>solved</t>
+  </si>
+  <si>
+    <t>this sum ko Solved karne ke baad he tujhe दोषमुक्त kahuga</t>
+  </si>
+  <si>
+    <t>अंतर्लीन करना(mela lena)</t>
+  </si>
+  <si>
+    <t>absorb</t>
+  </si>
+  <si>
+    <t>zoor</t>
+  </si>
+  <si>
+    <t>zoor se helane ke baad bhe cheeni chai me अंतर्लीन  nahi ho rahi hai</t>
+  </si>
+  <si>
+    <t>abstain</t>
+  </si>
+  <si>
+    <t>परहेज रखना</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>Train me alcohal pene se परहेज karna chaaheye.</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>track</t>
+  </si>
+  <si>
+    <t>ese track nahi kar sakte kyuki ye bahut he संक्षिप्त hai</t>
+  </si>
+  <si>
+    <t>absurd</t>
+  </si>
+  <si>
+    <t>बेतुका</t>
+  </si>
+  <si>
+    <t>sur of d</t>
+  </si>
+  <si>
+    <t>d ka sun बेतुका hai</t>
+  </si>
+  <si>
+    <t>accede</t>
+  </si>
+  <si>
+    <t>agree to</t>
+  </si>
+  <si>
+    <t>AC seed</t>
+  </si>
+  <si>
+    <t>AC me seed pak jaate hai, es baat par log hasne lage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accommodation </t>
+  </si>
+  <si>
+    <t>supply</t>
+  </si>
+  <si>
+    <t>AC morden</t>
+  </si>
+  <si>
+    <t>Morden AC ke supply nahi ho paa  rahi hai.</t>
+  </si>
+  <si>
+    <t>accompany</t>
+  </si>
+  <si>
+    <t>go with</t>
+  </si>
+  <si>
+    <t>I will go with my friend in AC company for interview</t>
+  </si>
+  <si>
+    <t>AC company</t>
+  </si>
+  <si>
+    <t>accursed</t>
+  </si>
+  <si>
+    <t>शापित</t>
+  </si>
+  <si>
+    <t>curse</t>
+  </si>
+  <si>
+    <t>accuse</t>
+  </si>
+  <si>
+    <t>दोष लगाना</t>
+  </si>
+  <si>
+    <t>AC ka use</t>
+  </si>
+  <si>
+    <t>AC ka use to karna aata nahi hai or ac company walon par दोष लगाना theek nahi ramu kaka</t>
+  </si>
+  <si>
+    <t>Acquaint</t>
+  </si>
+  <si>
+    <t>परिचित होना</t>
+  </si>
+  <si>
+    <t>ak aunty</t>
+  </si>
+  <si>
+    <t>ak aunty se mera परिचित kara do, jo mere help kar sake</t>
+  </si>
+  <si>
+    <t>Acquit</t>
+  </si>
+  <si>
+    <t>अपराधमुक्त करना</t>
+  </si>
+  <si>
+    <t>AC Quite</t>
+  </si>
+  <si>
+    <t>AC quite karke garmi me rahne se kya tum अपराधमुक्त ho jaaoge</t>
+  </si>
+  <si>
+    <t>A.D.</t>
+  </si>
+  <si>
+    <t>anno domini</t>
+  </si>
+  <si>
+    <t>Adamant</t>
+  </si>
+  <si>
+    <t>कठोर</t>
+  </si>
+  <si>
+    <t>aada+mint</t>
+  </si>
+  <si>
+    <t>Aada mint to bahut he कठोर hai</t>
+  </si>
+  <si>
+    <t>Adept</t>
+  </si>
+  <si>
+    <t>निपुण</t>
+  </si>
+  <si>
+    <t>adop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">everybody want to adop निपुण chield </t>
+  </si>
+  <si>
+    <t>adhere</t>
+  </si>
+  <si>
+    <t>Adver+here</t>
+  </si>
+  <si>
+    <t>चिपकना</t>
+  </si>
+  <si>
+    <t>Please Adver yahan(here) na चिपकना</t>
+  </si>
+  <si>
+    <t>adjoin</t>
+  </si>
+  <si>
+    <t>अगला होना</t>
+  </si>
+  <si>
+    <t>adver+join</t>
+  </si>
+  <si>
+    <t>अगला Adver yahan se join kar do</t>
+  </si>
+  <si>
+    <t>adjourn</t>
+  </si>
+  <si>
+    <t>टालना</t>
+  </si>
+  <si>
+    <t xml:space="preserve">additional+journy </t>
+  </si>
+  <si>
+    <t>Abhi additional journy ko टालना hoga,kyuki hamare pass time nahi hai.</t>
+  </si>
+  <si>
+    <t>admirable</t>
+  </si>
+  <si>
+    <t>admonish</t>
+  </si>
+  <si>
+    <t>adore</t>
+  </si>
+  <si>
+    <t>adverse</t>
+  </si>
+  <si>
+    <t>affection</t>
+  </si>
+  <si>
+    <t>affirm</t>
+  </si>
+  <si>
+    <t>affix</t>
+  </si>
+  <si>
+    <t>affluence</t>
+  </si>
+  <si>
+    <t>plenty</t>
+  </si>
+  <si>
+    <t>afresh</t>
+  </si>
+  <si>
+    <t>सराहनीय</t>
+  </si>
+  <si>
+    <t>admin+abality</t>
+  </si>
+  <si>
+    <t>system me admin ke abality सराहनीय hoti hai,use saar  power hote hai</t>
+  </si>
+  <si>
+    <t>धिक्कारना</t>
+  </si>
+  <si>
+    <t>ADD+manisha</t>
+  </si>
+  <si>
+    <t>manisha ne tujhe fb par nahi keya ye to धिक्कारना ho gaya</t>
+  </si>
+  <si>
+    <t>dhoor(animal)</t>
+  </si>
+  <si>
+    <t>बहुत चाहना</t>
+  </si>
+  <si>
+    <t>tu dhoor hai kya jo बहुत चाहना wali baate karta hai , samaajh bhi kuch hota hai ya nahi</t>
+  </si>
+  <si>
+    <t>विस्र्द्ध</t>
+  </si>
+  <si>
+    <t>Varsha(rain)</t>
+  </si>
+  <si>
+    <t>Vaarish k paani ke विस्र्द्ध koi kuch nahi kar sakta hai, ye to god ke he haath me hai</t>
+  </si>
+  <si>
+    <t>aerial</t>
+  </si>
+  <si>
+    <t>aerodroma</t>
+  </si>
+  <si>
+    <t>हवाई</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>mene real me हवाई yaatra ke hai</t>
+  </si>
+  <si>
+    <t>हवाई अड्डा</t>
+  </si>
+  <si>
+    <t>air+drama</t>
+  </si>
+  <si>
+    <t>Air me drama mat karo हवाई अड्डा par kar lena</t>
+  </si>
+  <si>
+    <t>ममता</t>
+  </si>
+  <si>
+    <t>infection</t>
+  </si>
+  <si>
+    <t>mujhe ममता infection ho gaya hai</t>
+  </si>
+  <si>
+    <t>विधिपूर्वक पुष्ट करना</t>
+  </si>
+  <si>
+    <t>farm</t>
+  </si>
+  <si>
+    <t>ye farm mera hai me eski विधिपूर्वक पुष्ट kar chuka hau</t>
+  </si>
+  <si>
+    <t>जोड़ना(attach)</t>
+  </si>
+  <si>
+    <t>Quice-fix</t>
+  </si>
+  <si>
+    <t>quice fix se kuch bhi जोड़ना nahi chaaheye</t>
+  </si>
+  <si>
+    <t>शिखर</t>
+  </si>
+  <si>
+    <t>flu</t>
+  </si>
+  <si>
+    <t>Flu aaj kal delhi me शिखर par hai</t>
+  </si>
+  <si>
+    <t>प्रचुरता</t>
+  </si>
+  <si>
+    <t>panty</t>
+  </si>
+  <si>
+    <t>ladies ke pass hamesha panty प्रचुरता me mil jaayegi</t>
+  </si>
+  <si>
+    <t>नए सिरे से</t>
+  </si>
+  <si>
+    <t>fresh</t>
+  </si>
+  <si>
+    <t>Fresh kaam hemesha नए सिरे से se karna chaaheye</t>
+  </si>
+  <si>
+    <t>abe DON ab to kaanoon ke aage give up kar de kyuki usne tujhe chaaron taraf se gher leya hai</t>
+  </si>
+  <si>
+    <t>1 mahan reshi ne yamuna nahi ko CURSE de kar use शापित kar deya hai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +637,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -98,6 +680,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="B1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1"/>
@@ -408,7 +992,7 @@
     <col min="8" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.95" customHeight="1">
+    <row r="1" spans="2:9" ht="24.95" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,36 +1010,702 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="24.95" customHeight="1">
-      <c r="A2">
-        <v>1</v>
-      </c>
+    <row r="2" spans="2:9" ht="24.95" customHeight="1">
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="24.95" customHeight="1">
+    <row r="3" spans="2:9" ht="24.95" customHeight="1">
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="24.95" customHeight="1">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="24.95" customHeight="1">
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="24.95" customHeight="1">
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" t="s">
+        <v>122</v>
+      </c>
+      <c r="E32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B36" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" t="s">
+        <v>136</v>
+      </c>
+      <c r="E36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" t="s">
+        <v>139</v>
+      </c>
+      <c r="E37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B38" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B39" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B40" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D40" t="s">
+        <v>161</v>
+      </c>
+      <c r="E40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B41" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D41" t="s">
+        <v>164</v>
+      </c>
+      <c r="E41" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B42" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D42" t="s">
+        <v>166</v>
+      </c>
+      <c r="E42" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B43" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D43" t="s">
+        <v>170</v>
+      </c>
+      <c r="E43" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" t="s">
+        <v>174</v>
+      </c>
+      <c r="D44" t="s">
+        <v>175</v>
+      </c>
+      <c r="E44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B45" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45" t="s">
+        <v>177</v>
+      </c>
+      <c r="D45" t="s">
+        <v>178</v>
+      </c>
+      <c r="E45" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B46" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D46" t="s">
+        <v>181</v>
+      </c>
+      <c r="E46" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B47" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D47" t="s">
+        <v>184</v>
+      </c>
+      <c r="E47" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B48" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D48" t="s">
+        <v>187</v>
+      </c>
+      <c r="E48" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B49" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" t="s">
+        <v>189</v>
+      </c>
+      <c r="D49" t="s">
+        <v>190</v>
+      </c>
+      <c r="E49" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B50" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D50" t="s">
+        <v>193</v>
+      </c>
+      <c r="E50" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B51" t="s">
+        <v>159</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D51" t="s">
+        <v>196</v>
+      </c>
+      <c r="E51" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -464,7 +1714,7 @@
     <mergeCell ref="E2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add memory key of words from at room at 23 jan 12
</commit_message>
<xml_diff>
--- a/Vocabulares.xlsx
+++ b/Vocabulares.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="697">
   <si>
     <t>Word</t>
   </si>
@@ -1303,13 +1303,817 @@
   </si>
   <si>
     <t>Has le jetna hasna hai has le tu apni धुरी par he rahega</t>
+  </si>
+  <si>
+    <t>granularity</t>
+  </si>
+  <si>
+    <t>दानेदार होना</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oversight </t>
+  </si>
+  <si>
+    <t>निरीक्षण</t>
+  </si>
+  <si>
+    <t>conveniently</t>
+  </si>
+  <si>
+    <t>सुविधा</t>
+  </si>
+  <si>
+    <t>compliment</t>
+  </si>
+  <si>
+    <t>प्रशंसा</t>
+  </si>
+  <si>
+    <t>complement</t>
+  </si>
+  <si>
+    <t>इज़ाफ़ा करना</t>
+  </si>
+  <si>
+    <t>comprise</t>
+  </si>
+  <si>
+    <t>शामिल करना</t>
+  </si>
+  <si>
+    <t>Compose</t>
+  </si>
+  <si>
+    <t>लिखना</t>
+  </si>
+  <si>
+    <t>concede</t>
+  </si>
+  <si>
+    <t>स्वीकार करना</t>
+  </si>
+  <si>
+    <t>concise</t>
+  </si>
+  <si>
+    <t>संक्षिप्त</t>
+  </si>
+  <si>
+    <t>Confer</t>
+  </si>
+  <si>
+    <t>प्रदान करना</t>
+  </si>
+  <si>
+    <t>connoisseur</t>
+  </si>
+  <si>
+    <t>विशेषज्ञ</t>
+  </si>
+  <si>
+    <t>Consist of</t>
+  </si>
+  <si>
+    <t>से मिलकर</t>
+  </si>
+  <si>
+    <t>Consist in</t>
+  </si>
+  <si>
+    <t>में शामिल</t>
+  </si>
+  <si>
+    <t>consistent</t>
+  </si>
+  <si>
+    <t>संगत</t>
+  </si>
+  <si>
+    <t>contagious</t>
+  </si>
+  <si>
+    <t>संक्रामक(pass by body)</t>
+  </si>
+  <si>
+    <t>infectious</t>
+  </si>
+  <si>
+    <t>संक्रामक(pass by air,water)</t>
+  </si>
+  <si>
+    <t>contemporary</t>
+  </si>
+  <si>
+    <t>समकालीन</t>
+  </si>
+  <si>
+    <t>contempt</t>
+  </si>
+  <si>
+    <t>तिरस्कार</t>
+  </si>
+  <si>
+    <t>Worthy</t>
+  </si>
+  <si>
+    <t>Continual</t>
+  </si>
+  <si>
+    <t>नित्य</t>
+  </si>
+  <si>
+    <t>convenience</t>
+  </si>
+  <si>
+    <t>cord</t>
+  </si>
+  <si>
+    <t>रस्सी</t>
+  </si>
+  <si>
+    <t>chord</t>
+  </si>
+  <si>
+    <t>तार</t>
+  </si>
+  <si>
+    <t>corporal punishment</t>
+  </si>
+  <si>
+    <t>शारीरिक दंड</t>
+  </si>
+  <si>
+    <t>barrister</t>
+  </si>
+  <si>
+    <t>बड़ा वकील</t>
+  </si>
+  <si>
+    <t>council</t>
+  </si>
+  <si>
+    <t>A COUNCIL is a board of elected representatives</t>
+  </si>
+  <si>
+    <t>counsel</t>
+  </si>
+  <si>
+    <t>Advice</t>
+  </si>
+  <si>
+    <t>counterfeit</t>
+  </si>
+  <si>
+    <t>जाली</t>
+  </si>
+  <si>
+    <t>courteous</t>
+  </si>
+  <si>
+    <t>विनम्र</t>
+  </si>
+  <si>
+    <t>credible</t>
+  </si>
+  <si>
+    <t>विश्वसनीय</t>
+  </si>
+  <si>
+    <t>crisis</t>
+  </si>
+  <si>
+    <t>संकट</t>
+  </si>
+  <si>
+    <t>criterion</t>
+  </si>
+  <si>
+    <t>कसौटी</t>
+  </si>
+  <si>
+    <t>criticise</t>
+  </si>
+  <si>
+    <t>आलोचना करना</t>
+  </si>
+  <si>
+    <t>crucial</t>
+  </si>
+  <si>
+    <t>महत्वपूर्ण</t>
+  </si>
+  <si>
+    <t>cupboard</t>
+  </si>
+  <si>
+    <t>अलमारी</t>
+  </si>
+  <si>
+    <t>curious</t>
+  </si>
+  <si>
+    <t>जिज्ञासु</t>
+  </si>
+  <si>
+    <t>curiosity</t>
+  </si>
+  <si>
+    <t>जिज्ञासा</t>
+  </si>
+  <si>
+    <t>currant</t>
+  </si>
+  <si>
+    <t>किशमिश</t>
+  </si>
+  <si>
+    <t>curriculum</t>
+  </si>
+  <si>
+    <t>कार्यक्रम</t>
+  </si>
+  <si>
+    <t>curriculum vitae</t>
+  </si>
+  <si>
+    <t>बायोडेटा</t>
+  </si>
+  <si>
+    <t>curtain</t>
+  </si>
+  <si>
+    <t>पर्दा</t>
+  </si>
+  <si>
+    <t>CERTAIN</t>
+  </si>
+  <si>
+    <t>पक्का</t>
+  </si>
+  <si>
+    <t>callous</t>
+  </si>
+  <si>
+    <t>निर्दयी</t>
+  </si>
+  <si>
+    <t>cannon</t>
+  </si>
+  <si>
+    <t>तोप</t>
+  </si>
+  <si>
+    <t>cleric</t>
+  </si>
+  <si>
+    <t>पुरोहित</t>
+  </si>
+  <si>
+    <t>caster</t>
+  </si>
+  <si>
+    <t>ढलाईकार</t>
+  </si>
+  <si>
+    <t>catarrh</t>
+  </si>
+  <si>
+    <t>नज़ला,सर्दी</t>
+  </si>
+  <si>
+    <t>ceiling</t>
+  </si>
+  <si>
+    <t>उच्चतम सीमा,छत</t>
+  </si>
+  <si>
+    <t>cereal</t>
+  </si>
+  <si>
+    <t>अनाज - संबंधी</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>धारावाहिक</t>
+  </si>
+  <si>
+    <t>ceremony</t>
+  </si>
+  <si>
+    <t>समारोह</t>
+  </si>
+  <si>
+    <t>childish</t>
+  </si>
+  <si>
+    <t>बचकाना</t>
+  </si>
+  <si>
+    <t>childlike</t>
+  </si>
+  <si>
+    <t>बच्चों का सा</t>
+  </si>
+  <si>
+    <t>coarse</t>
+  </si>
+  <si>
+    <t>गँवार</t>
+  </si>
+  <si>
+    <t>colossal</t>
+  </si>
+  <si>
+    <t>बहुत भारी</t>
+  </si>
+  <si>
+    <t>chasing</t>
+  </si>
+  <si>
+    <t>earnest</t>
+  </si>
+  <si>
+    <t>ईमानदार</t>
+  </si>
+  <si>
+    <t>eerie</t>
+  </si>
+  <si>
+    <t>भयानक</t>
+  </si>
+  <si>
+    <t>elude</t>
+  </si>
+  <si>
+    <t>embarrassing</t>
+  </si>
+  <si>
+    <t>शर्मनाक</t>
+  </si>
+  <si>
+    <t>emend</t>
+  </si>
+  <si>
+    <t>काट - छाँट करना</t>
+  </si>
+  <si>
+    <t>emphasise</t>
+  </si>
+  <si>
+    <t>ज़ोर देना</t>
+  </si>
+  <si>
+    <t>endeavour</t>
+  </si>
+  <si>
+    <t>प्रयास</t>
+  </si>
+  <si>
+    <t>enormity</t>
+  </si>
+  <si>
+    <t>महापाप</t>
+  </si>
+  <si>
+    <t>enquiry(british)</t>
+  </si>
+  <si>
+    <t>both are correct</t>
+  </si>
+  <si>
+    <t>Inquiry(American)</t>
+  </si>
+  <si>
+    <t>insure(arrange for financial)</t>
+  </si>
+  <si>
+    <t>ठीक कर लेना</t>
+  </si>
+  <si>
+    <t>ensure</t>
+  </si>
+  <si>
+    <t>सुनिश्चित करना</t>
+  </si>
+  <si>
+    <t>eventually</t>
+  </si>
+  <si>
+    <t>अंत में</t>
+  </si>
+  <si>
+    <t>EXHAUSTED</t>
+  </si>
+  <si>
+    <t>थका</t>
+  </si>
+  <si>
+    <t>exclaim</t>
+  </si>
+  <si>
+    <t>चिल्लाना</t>
+  </si>
+  <si>
+    <t>explicit</t>
+  </si>
+  <si>
+    <t>स्पष्ट</t>
+  </si>
+  <si>
+    <t>implicit</t>
+  </si>
+  <si>
+    <t>अस्पष्ट</t>
+  </si>
+  <si>
+    <t>extravagance</t>
+  </si>
+  <si>
+    <t>फिजूलखर्ची</t>
+  </si>
+  <si>
+    <t>ragularity</t>
+  </si>
+  <si>
+    <t>Ragularity chote -2 दानेदार step se banti hai.</t>
+  </si>
+  <si>
+    <t>Over+view</t>
+  </si>
+  <si>
+    <t>mene site ka over view karke pura निरीक्षण kar chuka hau.</t>
+  </si>
+  <si>
+    <t>Kon+evently</t>
+  </si>
+  <si>
+    <t>Kon se event सुविधा janak hai</t>
+  </si>
+  <si>
+    <t>Complant</t>
+  </si>
+  <si>
+    <t>Complant ke sabhi प्रशंसा karte hai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kam+emplement </t>
+  </si>
+  <si>
+    <t>Kam emplement karne se इज़ाफ़ा kam hota hai.</t>
+  </si>
+  <si>
+    <t>Kam+price</t>
+  </si>
+  <si>
+    <t>Kam price wali sabhi cheejaon ko list men शामिल mat karna.</t>
+  </si>
+  <si>
+    <t>kom+seed</t>
+  </si>
+  <si>
+    <t>Kon laya hai en seed ko ye स्वीकार nahi keye jaayenge.</t>
+  </si>
+  <si>
+    <t>kon+see+US</t>
+  </si>
+  <si>
+    <t>Kon US ko  संक्षिप्त me dekhna chaahta hai.</t>
+  </si>
+  <si>
+    <t>kon+prefer</t>
+  </si>
+  <si>
+    <t>kon prefer karega प्रदान karne ke leya.</t>
+  </si>
+  <si>
+    <t>Kon+serious</t>
+  </si>
+  <si>
+    <t>Kon sa  विशेषज्ञ serious apni thesis likhta hai.</t>
+  </si>
+  <si>
+    <t>Consist OFF</t>
+  </si>
+  <si>
+    <t>Consist से मिलकर OFF button banta hai.</t>
+  </si>
+  <si>
+    <t>Consist IN</t>
+  </si>
+  <si>
+    <t>Consist में शामिल hone k baad sabhi andar (IN) ho gate hai.</t>
+  </si>
+  <si>
+    <t>Assistant</t>
+  </si>
+  <si>
+    <t>Assistant ki संगतme mat rahna vo acchi ladki nahi hai.</t>
+  </si>
+  <si>
+    <t>continuous +genious</t>
+  </si>
+  <si>
+    <t>continuous genious 1 संक्रामक bemaari hai jo 1 body se dusari body jati hai</t>
+  </si>
+  <si>
+    <t>injuction</t>
+  </si>
+  <si>
+    <t>Injuction me water hota vo bhi hawa rahit</t>
+  </si>
+  <si>
+    <t>kom+temper</t>
+  </si>
+  <si>
+    <t>Kon ka temper bad raha hai jo तिरस्कार maag raha hai</t>
+  </si>
+  <si>
+    <t>Konse+tea+null</t>
+  </si>
+  <si>
+    <t>Konse se tea hamare NULL se nikalti hai</t>
+  </si>
+  <si>
+    <t>god</t>
+  </si>
+  <si>
+    <t>god tak jani ka rasta रस्सी hai</t>
+  </si>
+  <si>
+    <t>chod</t>
+  </si>
+  <si>
+    <t>Chodne ke leya तार ka kya kaam .</t>
+  </si>
+  <si>
+    <t>coparate+punishment</t>
+  </si>
+  <si>
+    <t>Coparate me  punishment शारीरिक दंड se roop me deya jata hai.</t>
+  </si>
+  <si>
+    <t>bade+sister</t>
+  </si>
+  <si>
+    <t>Meri badi sister बड़ा वकील hai ramghar me</t>
+  </si>
+  <si>
+    <t>Sell+kon</t>
+  </si>
+  <si>
+    <t>Sell karne k advice kon de raha hai tujhe</t>
+  </si>
+  <si>
+    <t>count+feet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unn feet ko count karo zin par जाली losain laga hua hai </t>
+  </si>
+  <si>
+    <t>court+us</t>
+  </si>
+  <si>
+    <t>court ne hame(us) विनम्र rahne ke war</t>
+  </si>
+  <si>
+    <t>Credit+available</t>
+  </si>
+  <si>
+    <t>Credit विश्वसनीय par he available hai</t>
+  </si>
+  <si>
+    <t>Krish+sis</t>
+  </si>
+  <si>
+    <t>Krish ke sis संकट me the touse bahut he gussa aagaya</t>
+  </si>
+  <si>
+    <t>Critariea</t>
+  </si>
+  <si>
+    <t>critariea ko cross karne par he asli insaan ke कसौटी hoti hai</t>
+  </si>
+  <si>
+    <t>critariea+size</t>
+  </si>
+  <si>
+    <t>critariea ka size bahut hi chota tha esi leye log meri आलोचना kar rahe the</t>
+  </si>
+  <si>
+    <t>tom crush+serial</t>
+  </si>
+  <si>
+    <t>tom crush serial bahut महत्वपूर्ण hai har 1 village me</t>
+  </si>
+  <si>
+    <t>cup+board</t>
+  </si>
+  <si>
+    <t>cup ko board ke bani अलमारी me rakh do</t>
+  </si>
+  <si>
+    <t>crush</t>
+  </si>
+  <si>
+    <t>crush par jaane ka mean  जिज्ञासु hau</t>
+  </si>
+  <si>
+    <t>curo+city</t>
+  </si>
+  <si>
+    <t>Curo city ke baare me meri janane ki जिज्ञासा bahut hai.</t>
+  </si>
+  <si>
+    <t>curent</t>
+  </si>
+  <si>
+    <t>Current lag jane par vykti ko किशमिश khelane chaaheye</t>
+  </si>
+  <si>
+    <t>kyu+ri+colum</t>
+  </si>
+  <si>
+    <t>Kyu ri tu apne colum me kyu nahi jati yaan beth kar कार्यक्रम kyu kahrab kar rahi hai</t>
+  </si>
+  <si>
+    <t>kyu+ri+colum+BEETA</t>
+  </si>
+  <si>
+    <t>Kyu ke colum ke beeta mela hai uska to ab CV life time ke keya gaya</t>
+  </si>
+  <si>
+    <t>Car+train</t>
+  </si>
+  <si>
+    <t>Car or train  k beech men पर्दा tha .</t>
+  </si>
+  <si>
+    <t>call+us</t>
+  </si>
+  <si>
+    <t>Call mat kayo us निर्दयी ko</t>
+  </si>
+  <si>
+    <t>CAN+ON</t>
+  </si>
+  <si>
+    <t>Kya koi on car(can) sakta hai तोप ko</t>
+  </si>
+  <si>
+    <t>clark</t>
+  </si>
+  <si>
+    <t>clark kabhi पुरोहित hua karte the kesi zammne me</t>
+  </si>
+  <si>
+    <t>Cast+kar</t>
+  </si>
+  <si>
+    <t>Cast banane walon kabhi ढलाईकार hua karte the kasi zamane mean.</t>
+  </si>
+  <si>
+    <t>Cat+harr</t>
+  </si>
+  <si>
+    <t>Cat ne harr kha le to use नज़ला,सर्दी ho gaya</t>
+  </si>
+  <si>
+    <t>seal</t>
+  </si>
+  <si>
+    <t>उच्चतम सीमा,छत par seal aa gayi hai</t>
+  </si>
+  <si>
+    <t>Serial</t>
+  </si>
+  <si>
+    <t>serial me अनाज - संबंधी baten bhi dekhayi jaayengi ye govt. se order hai</t>
+  </si>
+  <si>
+    <t>saari+monkey</t>
+  </si>
+  <si>
+    <t>Saare mokeies ka समारोह ho raha hai, pata nahi kya hoga</t>
+  </si>
+  <si>
+    <t>child+dish</t>
+  </si>
+  <si>
+    <t>Dish par child ke game dekhan bahut he बचकाना hai</t>
+  </si>
+  <si>
+    <t>child+like</t>
+  </si>
+  <si>
+    <t>child jesi like karte hai vo बच्चों का सा hai</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>Es course ko karne se गँवार bhi aachcha admi ban sakta hai.</t>
+  </si>
+  <si>
+    <t>cooles+saal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ye saal  cooles ke leya बहुत भारी hai </t>
+  </si>
+  <si>
+    <t>Chase</t>
+  </si>
+  <si>
+    <t>Chase me ghoda mera पीछा kar raha hai</t>
+  </si>
+  <si>
+    <t>year+next</t>
+  </si>
+  <si>
+    <t>Next year main me 1 ईमानदार insaan ban kar dekhauga</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>Ye area bahut he भयानक hai.</t>
+  </si>
+  <si>
+    <t>lequide</t>
+  </si>
+  <si>
+    <t>Im+bar+assian</t>
+  </si>
+  <si>
+    <t>I am bar assian karne wala hua ye 1 शर्मनाक kaam hai.</t>
+  </si>
+  <si>
+    <t>Im+end</t>
+  </si>
+  <si>
+    <t>I m end because mujhe laon se काट - छाँट kar thod deya hai.:tree</t>
+  </si>
+  <si>
+    <t>Im+phasise</t>
+  </si>
+  <si>
+    <t>I m living this phase. Tum es baat par kyu ज़ोर de rahe ho.</t>
+  </si>
+  <si>
+    <t>End+behaviour</t>
+  </si>
+  <si>
+    <t>End me behaviour badene ke  प्रयास se kuch nahi hota hai.</t>
+  </si>
+  <si>
+    <t>Ignore+amity</t>
+  </si>
+  <si>
+    <t>Amity university ko ignore karne ka महापाप kabhi mat karna</t>
+  </si>
+  <si>
+    <t>Event+actually</t>
+  </si>
+  <si>
+    <t>Actually me koi bhi अंत में excute nahi huyi.</t>
+  </si>
+  <si>
+    <t>Ex+air hoestest</t>
+  </si>
+  <si>
+    <t>Ex air hoestest me mujhe kal raat ko bahut thaka deya</t>
+  </si>
+  <si>
+    <t>claim</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Claim tumhe चिल्लाना se nahi mil jayega pahle ye form bharo</t>
+  </si>
+  <si>
+    <t>ex+city</t>
+  </si>
+  <si>
+    <t>Ye ex city se kitni स्पष्ट city hai na</t>
+  </si>
+  <si>
+    <t>Apple city nahut he अस्पष्ट hai, steav jobs k jaane k bad</t>
+  </si>
+  <si>
+    <t>apple+city</t>
+  </si>
+  <si>
+    <t>extra+reveange</t>
+  </si>
+  <si>
+    <t>Extra reveange me kuch nahi rakha hai ye sab फिजूलखर्ची hai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1344,6 +2148,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1371,7 +2183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1380,10 +2192,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1678,10 +2493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:I111"/>
+  <dimension ref="B1:I186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1"/>
@@ -1689,8 +2504,8 @@
     <col min="1" max="1" width="6.42578125" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="63.7109375" customWidth="1"/>
     <col min="8" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1704,13 +2519,13 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="2:9" ht="24.95" customHeight="1">
       <c r="B2" t="s">
@@ -1722,13 +2537,13 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="2:9" ht="24.95" customHeight="1">
       <c r="B3" t="s">
@@ -3217,6 +4032,972 @@
       </c>
       <c r="E111" t="s">
         <v>428</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" s="4" customFormat="1" ht="24.95" customHeight="1"/>
+    <row r="113" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B113" t="s">
+        <v>429</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="D113" t="s">
+        <v>572</v>
+      </c>
+      <c r="E113" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B114" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="D114" t="s">
+        <v>574</v>
+      </c>
+      <c r="E114" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B115" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C115" t="s">
+        <v>434</v>
+      </c>
+      <c r="D115" t="s">
+        <v>576</v>
+      </c>
+      <c r="E115" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B116" t="s">
+        <v>435</v>
+      </c>
+      <c r="C116" t="s">
+        <v>436</v>
+      </c>
+      <c r="D116" t="s">
+        <v>578</v>
+      </c>
+      <c r="E116" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B117" t="s">
+        <v>437</v>
+      </c>
+      <c r="C117" t="s">
+        <v>438</v>
+      </c>
+      <c r="D117" t="s">
+        <v>580</v>
+      </c>
+      <c r="E117" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B118" t="s">
+        <v>439</v>
+      </c>
+      <c r="C118" t="s">
+        <v>440</v>
+      </c>
+      <c r="D118" t="s">
+        <v>582</v>
+      </c>
+      <c r="E118" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B119" t="s">
+        <v>441</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B120" t="s">
+        <v>443</v>
+      </c>
+      <c r="C120" t="s">
+        <v>444</v>
+      </c>
+      <c r="D120" t="s">
+        <v>584</v>
+      </c>
+      <c r="E120" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B121" t="s">
+        <v>445</v>
+      </c>
+      <c r="C121" t="s">
+        <v>446</v>
+      </c>
+      <c r="D121" t="s">
+        <v>586</v>
+      </c>
+      <c r="E121" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B122" t="s">
+        <v>447</v>
+      </c>
+      <c r="C122" t="s">
+        <v>448</v>
+      </c>
+      <c r="D122" t="s">
+        <v>588</v>
+      </c>
+      <c r="E122" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B123" t="s">
+        <v>449</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="D123" t="s">
+        <v>590</v>
+      </c>
+      <c r="E123" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B124" t="s">
+        <v>451</v>
+      </c>
+      <c r="C124" t="s">
+        <v>452</v>
+      </c>
+      <c r="D124" t="s">
+        <v>592</v>
+      </c>
+      <c r="E124" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B125" t="s">
+        <v>453</v>
+      </c>
+      <c r="C125" t="s">
+        <v>454</v>
+      </c>
+      <c r="D125" t="s">
+        <v>594</v>
+      </c>
+      <c r="E125" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B126" t="s">
+        <v>455</v>
+      </c>
+      <c r="C126" t="s">
+        <v>456</v>
+      </c>
+      <c r="D126" t="s">
+        <v>596</v>
+      </c>
+      <c r="E126" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B127" t="s">
+        <v>457</v>
+      </c>
+      <c r="C127" t="s">
+        <v>458</v>
+      </c>
+      <c r="D127" t="s">
+        <v>598</v>
+      </c>
+      <c r="E127" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B128" t="s">
+        <v>459</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="D128" t="s">
+        <v>600</v>
+      </c>
+      <c r="E128" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B129" t="s">
+        <v>461</v>
+      </c>
+      <c r="C129" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B130" t="s">
+        <v>463</v>
+      </c>
+      <c r="C130" t="s">
+        <v>464</v>
+      </c>
+      <c r="D130" t="s">
+        <v>602</v>
+      </c>
+      <c r="E130" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B131" t="s">
+        <v>465</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B132" t="s">
+        <v>466</v>
+      </c>
+      <c r="C132" t="s">
+        <v>467</v>
+      </c>
+      <c r="D132" t="s">
+        <v>604</v>
+      </c>
+      <c r="E132" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B133" t="s">
+        <v>468</v>
+      </c>
+      <c r="C133" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B134" t="s">
+        <v>469</v>
+      </c>
+      <c r="C134" t="s">
+        <v>470</v>
+      </c>
+      <c r="D134" t="s">
+        <v>606</v>
+      </c>
+      <c r="E134" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B135" t="s">
+        <v>471</v>
+      </c>
+      <c r="C135" t="s">
+        <v>472</v>
+      </c>
+      <c r="D135" t="s">
+        <v>608</v>
+      </c>
+      <c r="E135" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B136" t="s">
+        <v>473</v>
+      </c>
+      <c r="C136" t="s">
+        <v>474</v>
+      </c>
+      <c r="D136" t="s">
+        <v>610</v>
+      </c>
+      <c r="E136" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B137" t="s">
+        <v>475</v>
+      </c>
+      <c r="C137" t="s">
+        <v>476</v>
+      </c>
+      <c r="D137" t="s">
+        <v>612</v>
+      </c>
+      <c r="E137" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B138" t="s">
+        <v>477</v>
+      </c>
+      <c r="C138" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B139" t="s">
+        <v>479</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="D139" t="s">
+        <v>614</v>
+      </c>
+      <c r="E139" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B140" t="s">
+        <v>481</v>
+      </c>
+      <c r="C140" t="s">
+        <v>482</v>
+      </c>
+      <c r="D140" t="s">
+        <v>616</v>
+      </c>
+      <c r="E140" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B141" t="s">
+        <v>483</v>
+      </c>
+      <c r="C141" t="s">
+        <v>484</v>
+      </c>
+      <c r="D141" t="s">
+        <v>618</v>
+      </c>
+      <c r="E141" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B142" t="s">
+        <v>485</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="D142" t="s">
+        <v>620</v>
+      </c>
+      <c r="E142" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B143" t="s">
+        <v>487</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="D143" t="s">
+        <v>622</v>
+      </c>
+      <c r="E143" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B144" t="s">
+        <v>489</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="D144" t="s">
+        <v>624</v>
+      </c>
+      <c r="E144" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B145" t="s">
+        <v>491</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="D145" t="s">
+        <v>626</v>
+      </c>
+      <c r="E145" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B146" t="s">
+        <v>493</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="D146" t="s">
+        <v>628</v>
+      </c>
+      <c r="E146" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B147" t="s">
+        <v>495</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="D147" t="s">
+        <v>630</v>
+      </c>
+      <c r="E147" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B148" t="s">
+        <v>497</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="D148" t="s">
+        <v>632</v>
+      </c>
+      <c r="E148" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B149" t="s">
+        <v>499</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="D149" t="s">
+        <v>634</v>
+      </c>
+      <c r="E149" s="10" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B150" t="s">
+        <v>501</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="D150" t="s">
+        <v>636</v>
+      </c>
+      <c r="E150" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B151" t="s">
+        <v>503</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="D151" t="s">
+        <v>638</v>
+      </c>
+      <c r="E151" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B152" t="s">
+        <v>505</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="D152" t="s">
+        <v>640</v>
+      </c>
+      <c r="E152" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B153" t="s">
+        <v>507</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="D153" t="s">
+        <v>642</v>
+      </c>
+      <c r="E153" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B154" t="s">
+        <v>509</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B155" t="s">
+        <v>511</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="D155" t="s">
+        <v>644</v>
+      </c>
+      <c r="E155" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="156" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B156" t="s">
+        <v>513</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="D156" t="s">
+        <v>646</v>
+      </c>
+      <c r="E156" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="157" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B157" t="s">
+        <v>515</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="D157" t="s">
+        <v>648</v>
+      </c>
+      <c r="E157" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="158" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B158" t="s">
+        <v>517</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="D158" t="s">
+        <v>650</v>
+      </c>
+      <c r="E158" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="159" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B159" t="s">
+        <v>519</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="D159" t="s">
+        <v>652</v>
+      </c>
+      <c r="E159" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="160" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B160" t="s">
+        <v>521</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="D160" t="s">
+        <v>654</v>
+      </c>
+      <c r="E160" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="161" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B161" t="s">
+        <v>523</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="D161" t="s">
+        <v>656</v>
+      </c>
+      <c r="E161" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="162" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B162" t="s">
+        <v>525</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="163" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B163" t="s">
+        <v>527</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="D163" t="s">
+        <v>658</v>
+      </c>
+      <c r="E163" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="164" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B164" t="s">
+        <v>529</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="D164" t="s">
+        <v>660</v>
+      </c>
+      <c r="E164" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="165" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B165" t="s">
+        <v>531</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="D165" t="s">
+        <v>662</v>
+      </c>
+      <c r="E165" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="166" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B166" t="s">
+        <v>533</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="D166" t="s">
+        <v>664</v>
+      </c>
+      <c r="E166" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="167" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B167" t="s">
+        <v>535</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="D167" t="s">
+        <v>666</v>
+      </c>
+      <c r="E167" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="168" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B168" t="s">
+        <v>537</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D168" t="s">
+        <v>668</v>
+      </c>
+      <c r="E168" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="169" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B169" t="s">
+        <v>538</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="D169" t="s">
+        <v>670</v>
+      </c>
+      <c r="E169" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="170" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B170" t="s">
+        <v>540</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="D170" t="s">
+        <v>672</v>
+      </c>
+      <c r="E170" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="171" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B171" t="s">
+        <v>542</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D171" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="172" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B172" t="s">
+        <v>543</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="D172" t="s">
+        <v>675</v>
+      </c>
+      <c r="E172" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="173" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B173" t="s">
+        <v>545</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="D173" t="s">
+        <v>677</v>
+      </c>
+      <c r="E173" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="174" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B174" t="s">
+        <v>547</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="D174" t="s">
+        <v>679</v>
+      </c>
+      <c r="E174" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="175" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B175" t="s">
+        <v>549</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="D175" t="s">
+        <v>681</v>
+      </c>
+      <c r="E175" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="176" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B176" t="s">
+        <v>551</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="D176" t="s">
+        <v>683</v>
+      </c>
+      <c r="E176" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="177" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B177" t="s">
+        <v>553</v>
+      </c>
+      <c r="C177" s="7" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="178" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B178" t="s">
+        <v>555</v>
+      </c>
+      <c r="C178" s="6"/>
+    </row>
+    <row r="179" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B179" t="s">
+        <v>556</v>
+      </c>
+      <c r="C179" s="7" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="180" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B180" t="s">
+        <v>558</v>
+      </c>
+      <c r="C180" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="181" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B181" t="s">
+        <v>560</v>
+      </c>
+      <c r="C181" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="D181" t="s">
+        <v>685</v>
+      </c>
+      <c r="E181" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="182" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B182" t="s">
+        <v>562</v>
+      </c>
+      <c r="C182" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="D182" t="s">
+        <v>687</v>
+      </c>
+      <c r="E182" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="183" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B183" t="s">
+        <v>564</v>
+      </c>
+      <c r="C183" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="D183" t="s">
+        <v>689</v>
+      </c>
+      <c r="E183" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="184" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B184" t="s">
+        <v>566</v>
+      </c>
+      <c r="C184" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="D184" t="s">
+        <v>691</v>
+      </c>
+      <c r="E184" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="185" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B185" t="s">
+        <v>568</v>
+      </c>
+      <c r="C185" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="D185" t="s">
+        <v>694</v>
+      </c>
+      <c r="E185" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="186" spans="2:5" ht="24.95" customHeight="1">
+      <c r="B186" t="s">
+        <v>570</v>
+      </c>
+      <c r="C186" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="D186" t="s">
+        <v>695</v>
+      </c>
+      <c r="E186" t="s">
+        <v>696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add some words without memory keys
</commit_message>
<xml_diff>
--- a/Vocabulares.xlsx
+++ b/Vocabulares.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="1035">
   <si>
     <t>Word</t>
   </si>
@@ -2058,9 +2058,6 @@
     <t>Event+actually</t>
   </si>
   <si>
-    <t>Actually me koi bhi अंत में excute nahi huyi.</t>
-  </si>
-  <si>
     <t>Ex+air hoestest</t>
   </si>
   <si>
@@ -2079,9 +2076,6 @@
     <t>Ye ex city se kitni स्पष्ट city hai na</t>
   </si>
   <si>
-    <t>Apple city nahut he अस्पष्ट hai, steav jobs k jaane k bad</t>
-  </si>
-  <si>
     <t>apple+city</t>
   </si>
   <si>
@@ -2194,15 +2188,6 @@
   </si>
   <si>
     <t>good+hand+sake</t>
-  </si>
-  <si>
-    <t>Logon ke भलाई के k leya ducket or pulish ne hand shake kar leya hai.</t>
-  </si>
-  <si>
-    <t>deap+see</t>
-  </si>
-  <si>
-    <t>Deap see me oxigen na milne par logo ko मृतक bana deya jata hai</t>
   </si>
   <si>
     <t>Dedi+sent</t>
@@ -2574,6 +2559,591 @@
   </si>
   <si>
     <t>Bear ka पीपा real me bhara rakha hua hai.</t>
+  </si>
+  <si>
+    <t>Deep see me oxigen na milne par logo ko मृतक bana deya jata hai</t>
+  </si>
+  <si>
+    <t>deep+see</t>
+  </si>
+  <si>
+    <t>Logon ke भलाई के k leya ducket or polish ne hand shake kar leya hai.</t>
+  </si>
+  <si>
+    <t>Apple city bahut he अस्पष्ट hai, steav jobs k jaane k bad</t>
+  </si>
+  <si>
+    <t>Actually me koi bhi  event अंत में excute nahi huyi.</t>
+  </si>
+  <si>
+    <t>Krish+sis</t>
+  </si>
+  <si>
+    <t>Immutable</t>
+  </si>
+  <si>
+    <t>अडिग</t>
+  </si>
+  <si>
+    <t>Mutable</t>
+  </si>
+  <si>
+    <t>परिवर्तनशील</t>
+  </si>
+  <si>
+    <t>demonstrates</t>
+  </si>
+  <si>
+    <t>यह दर्शाता है</t>
+  </si>
+  <si>
+    <t>explicitly</t>
+  </si>
+  <si>
+    <t>स्पष्ट रूप से</t>
+  </si>
+  <si>
+    <t>dame</t>
+  </si>
+  <si>
+    <t>married wonam</t>
+  </si>
+  <si>
+    <t>debate</t>
+  </si>
+  <si>
+    <t>वाद - विवाद</t>
+  </si>
+  <si>
+    <t>debt</t>
+  </si>
+  <si>
+    <t>उधार</t>
+  </si>
+  <si>
+    <t>decay</t>
+  </si>
+  <si>
+    <t>सड़ना</t>
+  </si>
+  <si>
+    <t>धोखा</t>
+  </si>
+  <si>
+    <t>deception(deceiving)</t>
+  </si>
+  <si>
+    <t>declare</t>
+  </si>
+  <si>
+    <t>स्पष्ट बता देना</t>
+  </si>
+  <si>
+    <t>dedication</t>
+  </si>
+  <si>
+    <t>समर्पण</t>
+  </si>
+  <si>
+    <t>deed</t>
+  </si>
+  <si>
+    <t>thing done</t>
+  </si>
+  <si>
+    <t>deform</t>
+  </si>
+  <si>
+    <t>बिगाड़ना</t>
+  </si>
+  <si>
+    <t>degenerate</t>
+  </si>
+  <si>
+    <t>हीन आदमी</t>
+  </si>
+  <si>
+    <t>नीचा दिखाना</t>
+  </si>
+  <si>
+    <t>degrade</t>
+  </si>
+  <si>
+    <t>प्रतिनिधि</t>
+  </si>
+  <si>
+    <t>delegate</t>
+  </si>
+  <si>
+    <t>deliberate</t>
+  </si>
+  <si>
+    <t>जानबूझकर</t>
+  </si>
+  <si>
+    <t>नाजुक</t>
+  </si>
+  <si>
+    <t>delicate</t>
+  </si>
+  <si>
+    <t>delight</t>
+  </si>
+  <si>
+    <t>सुख</t>
+  </si>
+  <si>
+    <t>demigod</t>
+  </si>
+  <si>
+    <t>उपदेवता</t>
+  </si>
+  <si>
+    <t>demolish</t>
+  </si>
+  <si>
+    <t>धूल में मिलाना</t>
+  </si>
+  <si>
+    <t>demon</t>
+  </si>
+  <si>
+    <t>राक्षस</t>
+  </si>
+  <si>
+    <t>denial</t>
+  </si>
+  <si>
+    <t>dense</t>
+  </si>
+  <si>
+    <t>घना</t>
+  </si>
+  <si>
+    <t>effigy</t>
+  </si>
+  <si>
+    <t>पुतला</t>
+  </si>
+  <si>
+    <t>elder</t>
+  </si>
+  <si>
+    <t>बड़ा</t>
+  </si>
+  <si>
+    <t>elevate</t>
+  </si>
+  <si>
+    <t>ऊपर उठाना</t>
+  </si>
+  <si>
+    <t>elope</t>
+  </si>
+  <si>
+    <t>फ़रार होना</t>
+  </si>
+  <si>
+    <t>संकट में डालना</t>
+  </si>
+  <si>
+    <t>embarrass</t>
+  </si>
+  <si>
+    <t>eminent</t>
+  </si>
+  <si>
+    <t>सुप्रसिद्ध</t>
+  </si>
+  <si>
+    <t>emphsis</t>
+  </si>
+  <si>
+    <t>ज़ोर</t>
+  </si>
+  <si>
+    <t>enact</t>
+  </si>
+  <si>
+    <t>क़ानून बनाना</t>
+  </si>
+  <si>
+    <t>enchant</t>
+  </si>
+  <si>
+    <t>मोहित करना</t>
+  </si>
+  <si>
+    <t>encounter</t>
+  </si>
+  <si>
+    <t>भिड़ंत</t>
+  </si>
+  <si>
+    <t>endurance</t>
+  </si>
+  <si>
+    <t>सहनशक्ति</t>
+  </si>
+  <si>
+    <t>endure</t>
+  </si>
+  <si>
+    <t>सहना</t>
+  </si>
+  <si>
+    <t>en mass</t>
+  </si>
+  <si>
+    <t>एक सामूहिक</t>
+  </si>
+  <si>
+    <t>enslave</t>
+  </si>
+  <si>
+    <t>ग़ुलाम बनाना</t>
+  </si>
+  <si>
+    <t>entangle</t>
+  </si>
+  <si>
+    <t>उलझाना</t>
+  </si>
+  <si>
+    <t>enthral</t>
+  </si>
+  <si>
+    <t>मोहित करन</t>
+  </si>
+  <si>
+    <t>entitle</t>
+  </si>
+  <si>
+    <t>समर्थ बनाना</t>
+  </si>
+  <si>
+    <t>entreat</t>
+  </si>
+  <si>
+    <t>गिड़गिड़ाना</t>
+  </si>
+  <si>
+    <t>entrust</t>
+  </si>
+  <si>
+    <t>सौंपना</t>
+  </si>
+  <si>
+    <t>envy</t>
+  </si>
+  <si>
+    <t>ईर्ष्या</t>
+  </si>
+  <si>
+    <t>epic</t>
+  </si>
+  <si>
+    <t>महाकाव्य</t>
+  </si>
+  <si>
+    <t>epidemic</t>
+  </si>
+  <si>
+    <t>महामारी</t>
+  </si>
+  <si>
+    <t>epoch</t>
+  </si>
+  <si>
+    <t>युग</t>
+  </si>
+  <si>
+    <t>fable</t>
+  </si>
+  <si>
+    <t>लघुकथा</t>
+  </si>
+  <si>
+    <t>fairy</t>
+  </si>
+  <si>
+    <t>परी</t>
+  </si>
+  <si>
+    <t>faith</t>
+  </si>
+  <si>
+    <t>विश्वास</t>
+  </si>
+  <si>
+    <t>trust,reliance</t>
+  </si>
+  <si>
+    <t>famine</t>
+  </si>
+  <si>
+    <t>अकाल</t>
+  </si>
+  <si>
+    <t>feast</t>
+  </si>
+  <si>
+    <t>feeble</t>
+  </si>
+  <si>
+    <t>कमजोर</t>
+  </si>
+  <si>
+    <t>feminine</t>
+  </si>
+  <si>
+    <t>women releated</t>
+  </si>
+  <si>
+    <t>fertile</t>
+  </si>
+  <si>
+    <t>उपजाऊ</t>
+  </si>
+  <si>
+    <t>fiction</t>
+  </si>
+  <si>
+    <t>उपन्यास</t>
+  </si>
+  <si>
+    <t>flesh</t>
+  </si>
+  <si>
+    <t>मांस</t>
+  </si>
+  <si>
+    <t>flee</t>
+  </si>
+  <si>
+    <t>भाग जाना</t>
+  </si>
+  <si>
+    <t>flaw</t>
+  </si>
+  <si>
+    <t>त्रुटि</t>
+  </si>
+  <si>
+    <t>flatter</t>
+  </si>
+  <si>
+    <t>चापलूसी करना</t>
+  </si>
+  <si>
+    <t>fling</t>
+  </si>
+  <si>
+    <t>फेंकान</t>
+  </si>
+  <si>
+    <t>flutter</t>
+  </si>
+  <si>
+    <t>फड़फड़ाहट</t>
+  </si>
+  <si>
+    <t>gaiety</t>
+  </si>
+  <si>
+    <t>खुशी</t>
+  </si>
+  <si>
+    <t>gallant(brave)</t>
+  </si>
+  <si>
+    <t>वीर</t>
+  </si>
+  <si>
+    <t>gallop</t>
+  </si>
+  <si>
+    <t>सरपट</t>
+  </si>
+  <si>
+    <t>gallows</t>
+  </si>
+  <si>
+    <t>फाँसी का तख़्ता</t>
+  </si>
+  <si>
+    <t>garland</t>
+  </si>
+  <si>
+    <t>फूलों की माला</t>
+  </si>
+  <si>
+    <t>garlic</t>
+  </si>
+  <si>
+    <t>लहसुन</t>
+  </si>
+  <si>
+    <t>gesture</t>
+  </si>
+  <si>
+    <t>हाव - भाव</t>
+  </si>
+  <si>
+    <t>giant</t>
+  </si>
+  <si>
+    <t>विशाल</t>
+  </si>
+  <si>
+    <t>ginger</t>
+  </si>
+  <si>
+    <t>अदरक</t>
+  </si>
+  <si>
+    <t>gist</t>
+  </si>
+  <si>
+    <t>निष्कर्ष</t>
+  </si>
+  <si>
+    <t>glance</t>
+  </si>
+  <si>
+    <t>झलक</t>
+  </si>
+  <si>
+    <t>glare</t>
+  </si>
+  <si>
+    <t>चमचमाना</t>
+  </si>
+  <si>
+    <t>glean</t>
+  </si>
+  <si>
+    <t>बटोरना</t>
+  </si>
+  <si>
+    <t>glimpse</t>
+  </si>
+  <si>
+    <t>झाँकी</t>
+  </si>
+  <si>
+    <t>glorious</t>
+  </si>
+  <si>
+    <t>प्रतापी,महान</t>
+  </si>
+  <si>
+    <t>glove</t>
+  </si>
+  <si>
+    <t>दस्ताना</t>
+  </si>
+  <si>
+    <t>hale</t>
+  </si>
+  <si>
+    <t>तन्दुरुस्त</t>
+  </si>
+  <si>
+    <t>halt</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>happen,occur</t>
+  </si>
+  <si>
+    <t>होना</t>
+  </si>
+  <si>
+    <t>harass</t>
+  </si>
+  <si>
+    <t>तंग करना</t>
+  </si>
+  <si>
+    <t>harbour</t>
+  </si>
+  <si>
+    <t>बन्दरगाह</t>
+  </si>
+  <si>
+    <t>haste</t>
+  </si>
+  <si>
+    <t>जल्दबाजी</t>
+  </si>
+  <si>
+    <t>hearth</t>
+  </si>
+  <si>
+    <t>चूल्हा</t>
+  </si>
+  <si>
+    <t>इसलिये</t>
+  </si>
+  <si>
+    <t>hence</t>
+  </si>
+  <si>
+    <t>झुंड</t>
+  </si>
+  <si>
+    <t>herd</t>
+  </si>
+  <si>
+    <t>आनुवंशिकता</t>
+  </si>
+  <si>
+    <t>heredity</t>
+  </si>
+  <si>
+    <t>बाधा</t>
+  </si>
+  <si>
+    <t>hindrance</t>
+  </si>
+  <si>
+    <t>मधुमुखी का छत्ता</t>
+  </si>
+  <si>
+    <t>hive</t>
+  </si>
+  <si>
+    <t>homage</t>
+  </si>
+  <si>
+    <t>श्रद्धांजलि</t>
+  </si>
+  <si>
+    <t>hoof</t>
+  </si>
+  <si>
+    <t>खुर</t>
+  </si>
+  <si>
+    <t>विरोधी</t>
+  </si>
+  <si>
+    <t>hostile</t>
+  </si>
+  <si>
+    <t>household</t>
+  </si>
+  <si>
+    <t>परिवार</t>
+  </si>
+  <si>
+    <t>humiliate</t>
+  </si>
+  <si>
+    <t>नीचा करना</t>
   </si>
 </sst>
 </file>
@@ -2662,7 +3232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2675,11 +3245,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2976,8 +3547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:I500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
-      <selection activeCell="E212" sqref="E212"/>
+    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="D342" sqref="D342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1"/>
@@ -3000,13 +3571,13 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
     </row>
     <row r="2" spans="2:9" ht="24.95" customHeight="1">
       <c r="B2" t="s">
@@ -3018,13 +3589,13 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="2:9" ht="24.95" customHeight="1">
       <c r="B3" t="s">
@@ -4535,7 +5106,7 @@
         <v>431</v>
       </c>
       <c r="C114" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>432</v>
@@ -4647,7 +5218,7 @@
         <v>448</v>
       </c>
       <c r="E122" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="123" spans="2:5" ht="24.95" customHeight="1">
@@ -4747,7 +5318,7 @@
         <v>463</v>
       </c>
       <c r="C130" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="D130" t="s">
         <v>464</v>
@@ -4775,7 +5346,7 @@
         <v>467</v>
       </c>
       <c r="E132" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="133" spans="2:5" ht="24.95" customHeight="1">
@@ -4889,7 +5460,7 @@
         <v>484</v>
       </c>
       <c r="E141" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="142" spans="2:5" ht="24.95" customHeight="1">
@@ -4911,7 +5482,7 @@
         <v>487</v>
       </c>
       <c r="C143" t="s">
-        <v>615</v>
+        <v>845</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>488</v>
@@ -5408,7 +5979,7 @@
         <v>561</v>
       </c>
       <c r="E181" t="s">
-        <v>680</v>
+        <v>844</v>
       </c>
     </row>
     <row r="182" spans="2:5" ht="24.95" customHeight="1">
@@ -5416,13 +5987,13 @@
         <v>562</v>
       </c>
       <c r="C182" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D182" s="7" t="s">
         <v>563</v>
       </c>
       <c r="E182" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="183" spans="2:5" ht="24.95" customHeight="1">
@@ -5430,13 +6001,13 @@
         <v>564</v>
       </c>
       <c r="C183" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D183" s="7" t="s">
         <v>565</v>
       </c>
       <c r="E183" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="184" spans="2:5" ht="24.95" customHeight="1">
@@ -5444,13 +6015,13 @@
         <v>566</v>
       </c>
       <c r="C184" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D184" s="7" t="s">
         <v>567</v>
       </c>
       <c r="E184" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="185" spans="2:5" ht="24.95" customHeight="1">
@@ -5458,13 +6029,13 @@
         <v>568</v>
       </c>
       <c r="C185" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="D185" s="7" t="s">
         <v>569</v>
       </c>
       <c r="E185" t="s">
-        <v>687</v>
+        <v>843</v>
       </c>
     </row>
     <row r="186" spans="2:5" ht="24.95" customHeight="1">
@@ -5472,334 +6043,334 @@
         <v>570</v>
       </c>
       <c r="C186" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D186" s="7" t="s">
         <v>571</v>
       </c>
       <c r="E186" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="187" spans="2:5" s="12" customFormat="1" ht="24.95" customHeight="1"/>
+        <v>688</v>
+      </c>
+    </row>
+    <row r="187" spans="2:5" s="10" customFormat="1" ht="24.95" customHeight="1"/>
     <row r="188" spans="2:5" ht="24.95" customHeight="1">
       <c r="B188" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D188" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="E188" t="s">
-        <v>726</v>
+        <v>842</v>
       </c>
     </row>
     <row r="189" spans="2:5" ht="24.95" customHeight="1">
       <c r="B189" s="5" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>727</v>
+        <v>841</v>
       </c>
       <c r="D189" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="E189" t="s">
-        <v>728</v>
+        <v>840</v>
       </c>
     </row>
     <row r="190" spans="2:5" ht="24.95" customHeight="1">
       <c r="B190" s="5" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="D190" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="191" spans="2:5" ht="24.95" customHeight="1">
       <c r="B191" s="5" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="C191" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="D191" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="E191" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
     </row>
     <row r="192" spans="2:5" ht="24.95" customHeight="1">
       <c r="B192" s="5" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D192" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="193" spans="2:5" ht="24.95" customHeight="1">
       <c r="B193" s="5" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="C193" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="D193" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="E193" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
     </row>
     <row r="194" spans="2:5" ht="24.95" customHeight="1">
       <c r="B194" s="5" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C194" s="3"/>
       <c r="D194" s="3" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="195" spans="2:5" ht="24.95" customHeight="1">
       <c r="B195" s="5" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C195" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="D195" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E195" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
     </row>
     <row r="196" spans="2:5" ht="24.95" customHeight="1">
       <c r="B196" s="5" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="C196" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="D196" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="E196" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
     </row>
     <row r="197" spans="2:5" ht="24.95" customHeight="1">
       <c r="B197" s="5" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="C197" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="D197" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="E197" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
     </row>
     <row r="198" spans="2:5" ht="24.95" customHeight="1">
       <c r="B198" s="5" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="D198" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="E198" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
     </row>
     <row r="199" spans="2:5" ht="24.95" customHeight="1">
       <c r="B199" s="5" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C199" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="D199" t="s">
         <v>232</v>
       </c>
       <c r="E199" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
     </row>
     <row r="200" spans="2:5" ht="24.95" customHeight="1">
       <c r="B200" s="5" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="C200" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="D200" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="E200" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
     </row>
     <row r="201" spans="2:5" ht="24.95" customHeight="1">
       <c r="B201" s="5" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="C201" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="D201" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E201" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
     </row>
     <row r="202" spans="2:5" ht="24.95" customHeight="1">
       <c r="B202" s="5" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C202" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="D202" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E202" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
     </row>
     <row r="203" spans="2:5" ht="24.95" customHeight="1">
       <c r="B203" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="C203" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
       <c r="D203" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="E203" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
     </row>
     <row r="204" spans="2:5" ht="24.95" customHeight="1">
       <c r="B204" s="5" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="C204" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
       <c r="D204" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="E204" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
     </row>
     <row r="205" spans="2:5" ht="24.95" customHeight="1">
       <c r="B205" s="5" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="C205" t="s">
-        <v>835</v>
+        <v>830</v>
       </c>
       <c r="D205" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="E205" t="s">
-        <v>836</v>
+        <v>831</v>
       </c>
     </row>
     <row r="206" spans="2:5" ht="24.95" customHeight="1">
       <c r="B206" s="5" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="C206" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
       <c r="E206" t="s">
-        <v>838</v>
+        <v>833</v>
       </c>
     </row>
     <row r="207" spans="2:5" ht="24.95" customHeight="1">
       <c r="B207" s="5" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
     </row>
     <row r="208" spans="2:5" ht="24.95" customHeight="1">
       <c r="B208" s="5" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
       <c r="C208" t="s">
-        <v>839</v>
+        <v>834</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>760</v>
+        <v>755</v>
       </c>
       <c r="E208" t="s">
-        <v>840</v>
+        <v>835</v>
       </c>
     </row>
     <row r="209" spans="2:5" ht="24.95" customHeight="1">
       <c r="B209" s="5" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="C209" t="s">
-        <v>841</v>
+        <v>836</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="E209" t="s">
-        <v>842</v>
+        <v>837</v>
       </c>
     </row>
     <row r="210" spans="2:5" ht="24.95" customHeight="1">
       <c r="B210" s="5" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="C210" t="s">
-        <v>843</v>
+        <v>838</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
       <c r="E210" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
     </row>
     <row r="211" spans="2:5" ht="24.95" customHeight="1">
       <c r="B211" s="5" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
     </row>
     <row r="212" spans="2:5" ht="24.95" customHeight="1">
       <c r="B212" s="5" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
     </row>
     <row r="213" spans="2:5" ht="24.95" customHeight="1">
       <c r="B213" s="5" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>269</v>
@@ -5807,250 +6378,1034 @@
     </row>
     <row r="214" spans="2:5" ht="24.95" customHeight="1">
       <c r="B214" s="5" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
     </row>
     <row r="215" spans="2:5" ht="24.95" customHeight="1">
       <c r="B215" s="5" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="216" spans="2:5" ht="24.95" customHeight="1">
       <c r="B216" s="5" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
     </row>
     <row r="217" spans="2:5" ht="24.95" customHeight="1">
       <c r="B217" s="5" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
     </row>
     <row r="218" spans="2:5" ht="24.95" customHeight="1">
       <c r="B218" s="5" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
     </row>
     <row r="219" spans="2:5" ht="24.95" customHeight="1">
       <c r="B219" s="5" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
     </row>
     <row r="220" spans="2:5" ht="24.95" customHeight="1">
       <c r="B220" s="5" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
     </row>
     <row r="221" spans="2:5" ht="24.95" customHeight="1">
       <c r="B221" s="5" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>784</v>
+        <v>779</v>
       </c>
     </row>
     <row r="222" spans="2:5" ht="24.95" customHeight="1">
       <c r="B222" s="5" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="D222" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
     </row>
     <row r="223" spans="2:5" ht="24.95" customHeight="1">
       <c r="B223" s="5" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
     </row>
     <row r="224" spans="2:5" ht="24.95" customHeight="1">
       <c r="B224" s="5" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>789</v>
+        <v>784</v>
       </c>
     </row>
     <row r="225" spans="2:4" ht="24.95" customHeight="1">
       <c r="B225" s="5" t="s">
-        <v>792</v>
+        <v>787</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
     </row>
     <row r="226" spans="2:4" ht="24.95" customHeight="1">
       <c r="B226" s="5" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
     </row>
     <row r="227" spans="2:4" ht="24.95" customHeight="1">
       <c r="B227" s="5" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
     </row>
     <row r="228" spans="2:4" ht="24.95" customHeight="1">
       <c r="B228" s="5" t="s">
-        <v>798</v>
+        <v>793</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="229" spans="2:4" ht="24.95" customHeight="1">
       <c r="B229" s="5" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>799</v>
+        <v>794</v>
       </c>
     </row>
     <row r="230" spans="2:4" ht="24.95" customHeight="1">
       <c r="B230" s="5" t="s">
-        <v>801</v>
+        <v>796</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
     </row>
     <row r="231" spans="2:4" ht="24.95" customHeight="1">
       <c r="B231" s="5" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
     </row>
     <row r="232" spans="2:4" ht="24.95" customHeight="1">
       <c r="B232" s="5" t="s">
-        <v>806</v>
+        <v>801</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
     </row>
     <row r="233" spans="2:4" ht="24.95" customHeight="1">
       <c r="B233" s="5" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
     </row>
     <row r="234" spans="2:4" ht="24.95" customHeight="1">
       <c r="B234" s="5" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
     </row>
     <row r="235" spans="2:4" ht="24.95" customHeight="1">
       <c r="B235" s="5" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
     </row>
     <row r="236" spans="2:4" ht="24.95" customHeight="1">
       <c r="B236" s="5" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
     </row>
     <row r="237" spans="2:4" ht="24.95" customHeight="1">
       <c r="B237" s="5" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
     </row>
     <row r="238" spans="2:4" ht="24.95" customHeight="1">
       <c r="B238" s="5" t="s">
-        <v>817</v>
+        <v>812</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>818</v>
+        <v>813</v>
       </c>
     </row>
     <row r="239" spans="2:4" ht="24.95" customHeight="1">
       <c r="B239" s="5" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>820</v>
+        <v>815</v>
       </c>
     </row>
     <row r="240" spans="2:4" ht="24.95" customHeight="1">
       <c r="B240" s="5" t="s">
-        <v>821</v>
+        <v>816</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>822</v>
+        <v>817</v>
       </c>
     </row>
     <row r="241" spans="2:4" ht="24.95" customHeight="1">
       <c r="B241" s="5" t="s">
-        <v>823</v>
+        <v>818</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>824</v>
+        <v>819</v>
       </c>
     </row>
     <row r="242" spans="2:4" ht="24.95" customHeight="1">
       <c r="B242" s="5" t="s">
-        <v>826</v>
+        <v>821</v>
       </c>
       <c r="D242" s="3" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
     </row>
     <row r="243" spans="2:4" ht="24.95" customHeight="1">
       <c r="B243" s="5" t="s">
-        <v>827</v>
+        <v>822</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>828</v>
+        <v>823</v>
       </c>
     </row>
     <row r="244" spans="2:4" ht="24.95" customHeight="1">
       <c r="B244" s="5" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>830</v>
+        <v>825</v>
+      </c>
+    </row>
+    <row r="245" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B245" s="5" t="s">
+        <v>846</v>
+      </c>
+      <c r="C245" s="3"/>
+      <c r="D245" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="246" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B246" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="C246" s="3"/>
+      <c r="D246" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="247" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B247" s="5" t="s">
+        <v>850</v>
+      </c>
+      <c r="D247" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="248" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B248" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="D248" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="249" spans="2:4" s="10" customFormat="1" ht="24.95" customHeight="1">
+      <c r="B249" s="11"/>
+    </row>
+    <row r="250" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B250" s="5" t="s">
+        <v>854</v>
+      </c>
+      <c r="D250" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="251" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B251" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="D251" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="252" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B252" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="D252" s="3" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="253" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B253" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="D253" s="3" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="254" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B254" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="D254" s="3" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="255" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B255" s="5" t="s">
+        <v>863</v>
+      </c>
+      <c r="D255" s="3" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="256" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B256" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="D256" s="3" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="257" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B257" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="D257" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="258" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B258" s="5" t="s">
+        <v>868</v>
+      </c>
+      <c r="D258" s="3" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="259" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B259" s="5" t="s">
+        <v>870</v>
+      </c>
+      <c r="D259" s="3" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="260" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B260" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="D260" s="3" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="261" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B261" s="5" t="s">
+        <v>875</v>
+      </c>
+      <c r="D261" s="3" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="262" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B262" s="5" t="s">
+        <v>877</v>
+      </c>
+      <c r="D262" s="3" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="263" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B263" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="D263" s="3" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="264" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B264" s="5" t="s">
+        <v>881</v>
+      </c>
+      <c r="D264" s="3" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="265" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B265" s="5" t="s">
+        <v>882</v>
+      </c>
+      <c r="D265" s="3" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="266" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B266" s="5" t="s">
+        <v>884</v>
+      </c>
+      <c r="D266" s="3" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="267" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B267" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="D267" s="3" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="268" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B268" s="5" t="s">
+        <v>888</v>
+      </c>
+      <c r="D268" s="3" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="269" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B269" s="5" t="s">
+        <v>890</v>
+      </c>
+      <c r="D269" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="270" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B270" s="5" t="s">
+        <v>891</v>
+      </c>
+      <c r="D270" s="3" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="271" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B271" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="D271" s="3" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="272" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B272" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="D272" s="3" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="273" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B273" s="5" t="s">
+        <v>897</v>
+      </c>
+      <c r="D273" s="3" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="274" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B274" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="D274" s="3" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="275" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B275" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="D275" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="276" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B276" s="5" t="s">
+        <v>902</v>
+      </c>
+      <c r="D276" s="3" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="277" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B277" s="5" t="s">
+        <v>903</v>
+      </c>
+      <c r="D277" s="3" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="278" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B278" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="D278" s="3" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="279" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B279" s="5" t="s">
+        <v>907</v>
+      </c>
+      <c r="D279" s="3" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="280" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B280" s="5" t="s">
+        <v>909</v>
+      </c>
+      <c r="D280" s="3" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="281" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B281" s="5" t="s">
+        <v>911</v>
+      </c>
+      <c r="D281" s="3" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="282" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B282" s="5" t="s">
+        <v>913</v>
+      </c>
+      <c r="D282" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="283" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B283" s="5" t="s">
+        <v>915</v>
+      </c>
+      <c r="D283" s="3" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="284" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B284" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="D284" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="285" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B285" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="D285" s="3" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="286" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B286" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="D286" s="3" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="287" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B287" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="D287" s="3" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="288" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B288" s="5" t="s">
+        <v>925</v>
+      </c>
+      <c r="D288" s="3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="289" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B289" s="5" t="s">
+        <v>927</v>
+      </c>
+      <c r="D289" s="3" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="290" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B290" s="5" t="s">
+        <v>929</v>
+      </c>
+      <c r="D290" s="3" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="291" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B291" s="5" t="s">
+        <v>931</v>
+      </c>
+      <c r="D291" s="3" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="292" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B292" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="D292" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="293" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B293" s="5" t="s">
+        <v>935</v>
+      </c>
+      <c r="D293" s="3" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="294" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B294" s="5" t="s">
+        <v>937</v>
+      </c>
+      <c r="D294" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="295" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B295" s="5" t="s">
+        <v>939</v>
+      </c>
+      <c r="D295" s="3" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="296" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B296" s="5" t="s">
+        <v>941</v>
+      </c>
+      <c r="D296" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="297" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B297" s="5" t="s">
+        <v>943</v>
+      </c>
+      <c r="C297" t="s">
+        <v>945</v>
+      </c>
+      <c r="D297" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="298" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B298" s="5" t="s">
+        <v>946</v>
+      </c>
+      <c r="D298" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="299" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B299" s="5" t="s">
+        <v>948</v>
+      </c>
+      <c r="D299" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="300" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B300" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="D300" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="301" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B301" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="D301" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="302" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B302" s="5" t="s">
+        <v>953</v>
+      </c>
+      <c r="D302" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="303" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B303" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="D303" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="304" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B304" s="5" t="s">
+        <v>957</v>
+      </c>
+      <c r="D304" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="305" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B305" s="5" t="s">
+        <v>959</v>
+      </c>
+      <c r="D305" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="306" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B306" s="5" t="s">
+        <v>961</v>
+      </c>
+      <c r="D306" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="307" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B307" s="5" t="s">
+        <v>963</v>
+      </c>
+      <c r="D307" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="308" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B308" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="D308" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="309" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B309" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="D309" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="310" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B310" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="D310" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="311" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B311" s="5" t="s">
+        <v>971</v>
+      </c>
+      <c r="D311" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="312" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B312" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="D312" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="313" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B313" s="5" t="s">
+        <v>975</v>
+      </c>
+      <c r="D313" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="314" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B314" s="5" t="s">
+        <v>977</v>
+      </c>
+      <c r="D314" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="315" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B315" s="5" t="s">
+        <v>979</v>
+      </c>
+      <c r="D315" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="316" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B316" s="5" t="s">
+        <v>981</v>
+      </c>
+      <c r="D316" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="317" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B317" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="D317" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="318" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B318" s="5" t="s">
+        <v>985</v>
+      </c>
+      <c r="D318" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="319" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B319" s="5" t="s">
+        <v>987</v>
+      </c>
+      <c r="D319" s="3" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="320" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B320" s="5" t="s">
+        <v>989</v>
+      </c>
+      <c r="D320" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="321" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B321" s="5" t="s">
+        <v>991</v>
+      </c>
+      <c r="D321" s="3" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="322" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B322" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="D322" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="323" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B323" s="5" t="s">
+        <v>995</v>
+      </c>
+      <c r="D323" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="324" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B324" s="5" t="s">
+        <v>997</v>
+      </c>
+      <c r="D324" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="325" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B325" s="5" t="s">
+        <v>999</v>
+      </c>
+      <c r="D325" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="326" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B326" s="5" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D326" s="3" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="327" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B327" s="5" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D327" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="328" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B328" s="5" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D328" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="329" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B329" s="5" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D329" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="330" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B330" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D330" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="331" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B331" s="5" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D331" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="332" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B332" s="5" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D332" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="333" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B333" s="5" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D333" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="334" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B334" s="5" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D334" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="335" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B335" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D335" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="336" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B336" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D336" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="337" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B337" s="5" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D337" s="3" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="338" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B338" s="5" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D338" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="339" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B339" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D339" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="340" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B340" s="5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D340" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="341" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B341" s="5" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D341" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="342" spans="2:4" ht="24.95" customHeight="1">
+      <c r="B342" s="5" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D342" t="s">
+        <v>1034</v>
       </c>
     </row>
     <row r="500" s="9" customFormat="1" ht="24.95" customHeight="1"/>

</xml_diff>

<commit_message>
Add some memory key form roo  on 27 jan 12
</commit_message>
<xml_diff>
--- a/Vocabulares.xlsx
+++ b/Vocabulares.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="1035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="1098">
   <si>
     <t>Word</t>
   </si>
@@ -3144,6 +3144,195 @@
   </si>
   <si>
     <t>नीचा करना</t>
+  </si>
+  <si>
+    <t>bhasker</t>
+  </si>
+  <si>
+    <t>Bhaskar धूप खाना ke leye apne chat par baitha hai.</t>
+  </si>
+  <si>
+    <t>Bee+get</t>
+  </si>
+  <si>
+    <t>Bee ko 1 ladki ko जन्म deya(get) hai</t>
+  </si>
+  <si>
+    <t>bee+seechaayi</t>
+  </si>
+  <si>
+    <t>Bee apne agricalchur form me seechayi(water) k leye प्रार्थना kar rahi hai.</t>
+  </si>
+  <si>
+    <t>Bee+side</t>
+  </si>
+  <si>
+    <t>Bee mere बगल में (side) me khaa gayi hai, ab bahut pain ho raha hai</t>
+  </si>
+  <si>
+    <t>bettry</t>
+  </si>
+  <si>
+    <t>Mere tourch ke bettry ne mujhe धोखा de deya</t>
+  </si>
+  <si>
+    <t>bilder</t>
+  </si>
+  <si>
+    <t>Bilder me mujhe उलझन में डाल deya kyuki usne mujhe bahut option deya hai</t>
+  </si>
+  <si>
+    <t>bid</t>
+  </si>
+  <si>
+    <t>blame+manisha</t>
+  </si>
+  <si>
+    <t>Manisha par blame laga deya ke charter par कलंक hai</t>
+  </si>
+  <si>
+    <t>blow+sun</t>
+  </si>
+  <si>
+    <t>Blow(under ground) mera sun फल - फूल raha hai</t>
+  </si>
+  <si>
+    <t>under</t>
+  </si>
+  <si>
+    <t>Under haath daal kar mene बड़ी भूल kar de</t>
+  </si>
+  <si>
+    <t>Bora</t>
+  </si>
+  <si>
+    <t>Bore me जंगली सूअर ko pakad kar band kar deya hai</t>
+  </si>
+  <si>
+    <t>batka</t>
+  </si>
+  <si>
+    <t>Abe batka karne ke leye tujhe चूतड़ he mela tha, ab office me sit kaise hunga</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>Uska land कुंद ho gaya hai</t>
+  </si>
+  <si>
+    <t>bhoopendar+chahra</t>
+  </si>
+  <si>
+    <t>Bhoopendar ka chahra कसाई k jaisa hai</t>
+  </si>
+  <si>
+    <t>bhoory</t>
+  </si>
+  <si>
+    <t>bhoory ke दफनाना k leye kabreestaan me jagha nahi mele.</t>
+  </si>
+  <si>
+    <t>bhory+kal</t>
+  </si>
+  <si>
+    <t>Bhoory ko kal दफन keya jaayega</t>
+  </si>
+  <si>
+    <t>brushli+taal</t>
+  </si>
+  <si>
+    <t>brushli ke karate wali taal bahut निर्दय hai</t>
+  </si>
+  <si>
+    <t>brick</t>
+  </si>
+  <si>
+    <t>Brick ko break karne le फुर्तीला hona bahut zaroori hai</t>
+  </si>
+  <si>
+    <t>rim</t>
+  </si>
+  <si>
+    <t>mere cycle ke rim ke किनारा par lahag aa gayi hai</t>
+  </si>
+  <si>
+    <t>battel</t>
+  </si>
+  <si>
+    <t>Battel me kuch bhi भुरभुरा nahi hota hai</t>
+  </si>
+  <si>
+    <t>bra+bibi ka</t>
+  </si>
+  <si>
+    <t>Bibi ka bra kharidne ke leya bhi mujhe रिशवत  deni padi hai</t>
+  </si>
+  <si>
+    <t>break+down</t>
+  </si>
+  <si>
+    <t>Pattar break karke road pe neeche(down) phek do</t>
+  </si>
+  <si>
+    <t>beach</t>
+  </si>
+  <si>
+    <t>beach par agar rule break keya to samjhe tum mare gayi</t>
+  </si>
+  <si>
+    <t>bread</t>
+  </si>
+  <si>
+    <t>bread ko चोटी me laga kar market me ghoomna chaaheye</t>
+  </si>
+  <si>
+    <t>wo</t>
+  </si>
+  <si>
+    <t>Wo wali डाल katni  hai</t>
+  </si>
+  <si>
+    <t>Boss+mein</t>
+  </si>
+  <si>
+    <t>Boss main hau to meri छाती kar kyu chad rahe ho</t>
+  </si>
+  <si>
+    <t>bone</t>
+  </si>
+  <si>
+    <t>Bone sahi hone ka वरदान tuto he milna chaheya.</t>
+  </si>
+  <si>
+    <t>Book+worm</t>
+  </si>
+  <si>
+    <t>Boom me worm pad gaye hai ye पुस्ताकों का कीड़ा hai</t>
+  </si>
+  <si>
+    <t>mute+table</t>
+  </si>
+  <si>
+    <t>Mute table ko koi hela nahi sakta wo अडिग hai</t>
+  </si>
+  <si>
+    <t>moot(pee)</t>
+  </si>
+  <si>
+    <t>Moot karne ke leya परिवर्तनशील hona he padta hai, warna…</t>
+  </si>
+  <si>
+    <t>Demo+street</t>
+  </si>
+  <si>
+    <t>Street  par demo dekhana यह दर्शाता है hai ke bande me koi baat nahi nai</t>
+  </si>
+  <si>
+    <t>explain+city</t>
+  </si>
+  <si>
+    <t>Explain karo स्पष्ट रूप से this city ko, jahan par tum rahte ho</t>
   </si>
 </sst>
 </file>
@@ -3194,7 +3383,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3219,6 +3408,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3232,7 +3427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3251,6 +3446,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3545,10 +3741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:I500"/>
+  <dimension ref="A1:I500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
-      <selection activeCell="D342" sqref="D342"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="E248" sqref="E248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1"/>
@@ -3557,7 +3753,7 @@
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="63.7109375" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" customWidth="1"/>
     <col min="8" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6324,7 +6520,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="209" spans="2:5" ht="24.95" customHeight="1">
+    <row r="209" spans="1:5" ht="24.95" customHeight="1">
       <c r="B209" s="5" t="s">
         <v>756</v>
       </c>
@@ -6338,7 +6534,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="210" spans="2:5" ht="24.95" customHeight="1">
+    <row r="210" spans="1:5" ht="24.95" customHeight="1">
       <c r="B210" s="5" t="s">
         <v>759</v>
       </c>
@@ -6352,71 +6548,119 @@
         <v>839</v>
       </c>
     </row>
-    <row r="211" spans="2:5" ht="24.95" customHeight="1">
+    <row r="211" spans="1:5" ht="24.95" customHeight="1">
       <c r="B211" s="5" t="s">
         <v>760</v>
       </c>
+      <c r="C211" t="s">
+        <v>1035</v>
+      </c>
       <c r="D211" s="3" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="212" spans="2:5" ht="24.95" customHeight="1">
+      <c r="E211" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" ht="24.95" customHeight="1">
       <c r="B212" s="5" t="s">
         <v>762</v>
       </c>
+      <c r="C212" t="s">
+        <v>1037</v>
+      </c>
       <c r="D212" s="3" t="s">
         <v>763</v>
       </c>
-    </row>
-    <row r="213" spans="2:5" ht="24.95" customHeight="1">
+      <c r="E212" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" ht="24.95" customHeight="1">
       <c r="B213" s="5" t="s">
         <v>764</v>
       </c>
+      <c r="C213" t="s">
+        <v>1039</v>
+      </c>
       <c r="D213" s="3" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="214" spans="2:5" ht="24.95" customHeight="1">
+      <c r="E213" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" ht="24.95" customHeight="1">
       <c r="B214" s="5" t="s">
         <v>766</v>
       </c>
+      <c r="C214" t="s">
+        <v>1041</v>
+      </c>
       <c r="D214" s="3" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="215" spans="2:5" ht="24.95" customHeight="1">
+      <c r="E214" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" ht="24.95" customHeight="1">
       <c r="B215" s="5" t="s">
         <v>767</v>
       </c>
+      <c r="C215" t="s">
+        <v>1043</v>
+      </c>
       <c r="D215" s="3" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="216" spans="2:5" ht="24.95" customHeight="1">
+      <c r="E215" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" ht="24.95" customHeight="1">
       <c r="B216" s="5" t="s">
         <v>769</v>
       </c>
+      <c r="C216" t="s">
+        <v>1045</v>
+      </c>
       <c r="D216" s="3" t="s">
         <v>768</v>
       </c>
-    </row>
-    <row r="217" spans="2:5" ht="24.95" customHeight="1">
+      <c r="E216" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" ht="24.95" customHeight="1">
       <c r="B217" s="5" t="s">
         <v>770</v>
       </c>
+      <c r="C217" t="s">
+        <v>1047</v>
+      </c>
       <c r="D217" s="3" t="s">
         <v>771</v>
       </c>
-    </row>
-    <row r="218" spans="2:5" ht="24.95" customHeight="1">
+      <c r="E217" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" ht="24.95" customHeight="1">
       <c r="B218" s="5" t="s">
         <v>773</v>
       </c>
+      <c r="C218" t="s">
+        <v>1048</v>
+      </c>
       <c r="D218" s="3" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="219" spans="2:5" ht="24.95" customHeight="1">
+      <c r="E218" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" ht="24.95" customHeight="1">
       <c r="B219" s="5" t="s">
         <v>774</v>
       </c>
@@ -6424,31 +6668,50 @@
         <v>775</v>
       </c>
     </row>
-    <row r="220" spans="2:5" ht="24.95" customHeight="1">
+    <row r="220" spans="1:5" ht="24.95" customHeight="1">
       <c r="B220" s="5" t="s">
         <v>777</v>
       </c>
+      <c r="C220" t="s">
+        <v>1050</v>
+      </c>
       <c r="D220" s="3" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="221" spans="2:5" ht="24.95" customHeight="1">
+      <c r="E220" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" ht="24.95" customHeight="1">
       <c r="B221" s="5" t="s">
         <v>778</v>
       </c>
+      <c r="C221" t="s">
+        <v>1052</v>
+      </c>
       <c r="D221" s="3" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="222" spans="2:5" ht="24.95" customHeight="1">
+      <c r="E221" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" ht="24.95" customHeight="1">
       <c r="B222" s="5" t="s">
         <v>780</v>
       </c>
+      <c r="C222" t="s">
+        <v>1058</v>
+      </c>
       <c r="D222" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="223" spans="2:5" ht="24.95" customHeight="1">
+      <c r="E222" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A223" s="14"/>
       <c r="B223" s="5" t="s">
         <v>783</v>
       </c>
@@ -6456,47 +6719,77 @@
         <v>782</v>
       </c>
     </row>
-    <row r="224" spans="2:5" ht="24.95" customHeight="1">
+    <row r="224" spans="1:5" ht="24.95" customHeight="1">
       <c r="B224" s="5" t="s">
         <v>785</v>
       </c>
+      <c r="C224" t="s">
+        <v>1054</v>
+      </c>
       <c r="D224" s="3" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="225" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E224" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="225" spans="2:5" ht="24.95" customHeight="1">
       <c r="B225" s="5" t="s">
         <v>787</v>
       </c>
+      <c r="C225" t="s">
+        <v>1056</v>
+      </c>
       <c r="D225" s="3" t="s">
         <v>786</v>
       </c>
-    </row>
-    <row r="226" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E225" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="226" spans="2:5" ht="24.95" customHeight="1">
       <c r="B226" s="5" t="s">
         <v>789</v>
       </c>
+      <c r="C226" t="s">
+        <v>1060</v>
+      </c>
       <c r="D226" s="3" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="227" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E226" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="227" spans="2:5" ht="24.95" customHeight="1">
       <c r="B227" s="5" t="s">
         <v>791</v>
       </c>
+      <c r="C227" t="s">
+        <v>1062</v>
+      </c>
       <c r="D227" s="3" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="228" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E227" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="228" spans="2:5" ht="24.95" customHeight="1">
       <c r="B228" s="5" t="s">
         <v>793</v>
       </c>
+      <c r="C228" t="s">
+        <v>1064</v>
+      </c>
       <c r="D228" s="3" t="s">
         <v>792</v>
       </c>
-    </row>
-    <row r="229" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E228" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="229" spans="2:5" ht="24.95" customHeight="1">
       <c r="B229" s="5" t="s">
         <v>795</v>
       </c>
@@ -6504,7 +6797,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="230" spans="2:4" ht="24.95" customHeight="1">
+    <row r="230" spans="2:5" ht="24.95" customHeight="1">
       <c r="B230" s="5" t="s">
         <v>796</v>
       </c>
@@ -6512,39 +6805,63 @@
         <v>797</v>
       </c>
     </row>
-    <row r="231" spans="2:4" ht="24.95" customHeight="1">
+    <row r="231" spans="2:5" ht="24.95" customHeight="1">
       <c r="B231" s="5" t="s">
         <v>799</v>
       </c>
+      <c r="C231" t="s">
+        <v>1066</v>
+      </c>
       <c r="D231" s="3" t="s">
         <v>798</v>
       </c>
-    </row>
-    <row r="232" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E231" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="232" spans="2:5" ht="24.95" customHeight="1">
       <c r="B232" s="5" t="s">
         <v>801</v>
       </c>
+      <c r="C232" t="s">
+        <v>1072</v>
+      </c>
       <c r="D232" s="3" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="233" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E232" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="233" spans="2:5" ht="24.95" customHeight="1">
       <c r="B233" s="5" t="s">
         <v>803</v>
       </c>
+      <c r="C233" t="s">
+        <v>1068</v>
+      </c>
       <c r="D233" s="3" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="234" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E233" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="234" spans="2:5" ht="24.95" customHeight="1">
       <c r="B234" s="5" t="s">
         <v>805</v>
       </c>
+      <c r="C234" t="s">
+        <v>1070</v>
+      </c>
       <c r="D234" s="3" t="s">
         <v>804</v>
       </c>
-    </row>
-    <row r="235" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E234" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="235" spans="2:5" ht="24.95" customHeight="1">
       <c r="B235" s="5" t="s">
         <v>806</v>
       </c>
@@ -6552,7 +6869,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="236" spans="2:4" ht="24.95" customHeight="1">
+    <row r="236" spans="2:5" ht="24.95" customHeight="1">
       <c r="B236" s="5" t="s">
         <v>808</v>
       </c>
@@ -6560,108 +6877,178 @@
         <v>809</v>
       </c>
     </row>
-    <row r="237" spans="2:4" ht="24.95" customHeight="1">
+    <row r="237" spans="2:5" ht="24.95" customHeight="1">
       <c r="B237" s="5" t="s">
         <v>810</v>
       </c>
+      <c r="C237" t="s">
+        <v>1074</v>
+      </c>
       <c r="D237" s="3" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="238" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E237" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="238" spans="2:5" ht="24.95" customHeight="1">
       <c r="B238" s="5" t="s">
         <v>812</v>
       </c>
+      <c r="C238" t="s">
+        <v>1076</v>
+      </c>
       <c r="D238" s="3" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="239" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E238" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="239" spans="2:5" ht="24.95" customHeight="1">
       <c r="B239" s="5" t="s">
         <v>814</v>
       </c>
+      <c r="C239" t="s">
+        <v>1078</v>
+      </c>
       <c r="D239" s="3" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="240" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E239" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="240" spans="2:5" ht="24.95" customHeight="1">
       <c r="B240" s="5" t="s">
         <v>816</v>
       </c>
+      <c r="C240" t="s">
+        <v>1080</v>
+      </c>
       <c r="D240" s="3" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="241" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E240" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="241" spans="2:5" ht="24.95" customHeight="1">
       <c r="B241" s="5" t="s">
         <v>818</v>
       </c>
+      <c r="C241" t="s">
+        <v>1082</v>
+      </c>
       <c r="D241" s="3" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="242" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E241" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="242" spans="2:5" ht="24.95" customHeight="1">
       <c r="B242" s="5" t="s">
         <v>821</v>
       </c>
+      <c r="C242" t="s">
+        <v>1084</v>
+      </c>
       <c r="D242" s="3" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="243" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E242" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="243" spans="2:5" ht="24.95" customHeight="1">
       <c r="B243" s="5" t="s">
         <v>822</v>
       </c>
+      <c r="C243" t="s">
+        <v>1086</v>
+      </c>
       <c r="D243" s="3" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="244" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E243" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="244" spans="2:5" ht="24.95" customHeight="1">
       <c r="B244" s="5" t="s">
         <v>824</v>
       </c>
+      <c r="C244" t="s">
+        <v>1088</v>
+      </c>
       <c r="D244" s="3" t="s">
         <v>825</v>
       </c>
-    </row>
-    <row r="245" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E244" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="245" spans="2:5" ht="24.95" customHeight="1">
       <c r="B245" s="5" t="s">
         <v>846</v>
       </c>
-      <c r="C245" s="3"/>
+      <c r="C245" s="3" t="s">
+        <v>1090</v>
+      </c>
       <c r="D245" t="s">
         <v>847</v>
       </c>
-    </row>
-    <row r="246" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E245" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="246" spans="2:5" ht="24.95" customHeight="1">
       <c r="B246" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="C246" s="3"/>
+      <c r="C246" s="3" t="s">
+        <v>1092</v>
+      </c>
       <c r="D246" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="247" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E246" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="247" spans="2:5" ht="24.95" customHeight="1">
       <c r="B247" s="5" t="s">
         <v>850</v>
       </c>
+      <c r="C247" t="s">
+        <v>1094</v>
+      </c>
       <c r="D247" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="248" spans="2:4" ht="24.95" customHeight="1">
+      <c r="E247" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="248" spans="2:5" ht="24.95" customHeight="1">
       <c r="B248" s="5" t="s">
         <v>852</v>
       </c>
+      <c r="C248" t="s">
+        <v>1096</v>
+      </c>
       <c r="D248" t="s">
         <v>853</v>
       </c>
-    </row>
-    <row r="249" spans="2:4" s="10" customFormat="1" ht="24.95" customHeight="1">
+      <c r="E248" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="249" spans="2:5" s="10" customFormat="1" ht="24.95" customHeight="1">
       <c r="B249" s="11"/>
     </row>
-    <row r="250" spans="2:4" ht="24.95" customHeight="1">
+    <row r="250" spans="2:5" ht="24.95" customHeight="1">
       <c r="B250" s="5" t="s">
         <v>854</v>
       </c>
@@ -6669,7 +7056,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="251" spans="2:4" ht="24.95" customHeight="1">
+    <row r="251" spans="2:5" ht="24.95" customHeight="1">
       <c r="B251" s="5" t="s">
         <v>856</v>
       </c>
@@ -6677,7 +7064,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="252" spans="2:4" ht="24.95" customHeight="1">
+    <row r="252" spans="2:5" ht="24.95" customHeight="1">
       <c r="B252" s="5" t="s">
         <v>858</v>
       </c>
@@ -6685,7 +7072,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="253" spans="2:4" ht="24.95" customHeight="1">
+    <row r="253" spans="2:5" ht="24.95" customHeight="1">
       <c r="B253" s="5" t="s">
         <v>860</v>
       </c>
@@ -6693,7 +7080,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="254" spans="2:4" ht="24.95" customHeight="1">
+    <row r="254" spans="2:5" ht="24.95" customHeight="1">
       <c r="B254" s="5" t="s">
         <v>704</v>
       </c>
@@ -6701,7 +7088,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="255" spans="2:4" ht="24.95" customHeight="1">
+    <row r="255" spans="2:5" ht="24.95" customHeight="1">
       <c r="B255" s="5" t="s">
         <v>863</v>
       </c>
@@ -6709,7 +7096,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="256" spans="2:4" ht="24.95" customHeight="1">
+    <row r="256" spans="2:5" ht="24.95" customHeight="1">
       <c r="B256" s="5" t="s">
         <v>864</v>
       </c>

</xml_diff>